<commit_message>
After updating profiles with global variables
</commit_message>
<xml_diff>
--- a/Data Files/CheckpointsData.xlsx
+++ b/Data Files/CheckpointsData.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>UserID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Password</t>
   </si>
@@ -27,13 +24,28 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t xml:space="preserve">John </t>
-  </si>
-  <si>
     <t>ThisIsNotAPassword</t>
   </si>
   <si>
-    <t>ThisIsNot</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Invalid UserName</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>Appointment Date</t>
+  </si>
+  <si>
+    <t>John DO</t>
+  </si>
+  <si>
+    <t>ThisIsNotPass</t>
+  </si>
+  <si>
+    <t>John Test1</t>
   </si>
 </sst>
 </file>
@@ -69,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,52 +385,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44684</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="John@"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>